<commit_message>
Updated names to more descriptive format. Might still need to update files to reflect name changes.
</commit_message>
<xml_diff>
--- a/soil_otu_activity_pattern/sortedotus.xlsx
+++ b/soil_otu_activity_pattern/sortedotus.xlsx
@@ -1,33 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mstate-my.sharepoint.com/personal/ts2492_msstate_edu/Documents/Research/Microbial ecology/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tj/git/ul-spacetime/soil_otu_activity_pattern/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{5138BBEA-98C8-BE41-AAE4-37B37998BD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{527DE69F-1913-FD4C-BA07-B86EC82722A7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10F9C94-07C0-6D4F-A587-CE24AADE54D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D9EB2712-0AFE-9649-8312-B232512868FA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" firstSheet="1" activeTab="7" xr2:uid="{D9EB2712-0AFE-9649-8312-B232512868FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
     <sheet name="DNA" sheetId="1" r:id="rId2"/>
-    <sheet name="ul.dna.soilotus.s3" sheetId="8" r:id="rId3"/>
-    <sheet name="ul.dna.soilotus.s2" sheetId="7" r:id="rId4"/>
-    <sheet name="ul.dna.soilotus.s1" sheetId="6" r:id="rId5"/>
-    <sheet name="ul.dna.soilotus.fh" sheetId="5" r:id="rId6"/>
-    <sheet name="ul.dna.soilotus.always" sheetId="2" r:id="rId7"/>
-    <sheet name="ul.dna.soilotus.blips" sheetId="4" r:id="rId8"/>
+    <sheet name="timeseries.soil.otus.dna.s3" sheetId="8" r:id="rId3"/>
+    <sheet name="timeseries.soil.otus.dna.s2" sheetId="7" r:id="rId4"/>
+    <sheet name="timeseries.soil.otus.dna.s1" sheetId="6" r:id="rId5"/>
+    <sheet name="timeseries.soil.otus.dna.fh" sheetId="5" r:id="rId6"/>
+    <sheet name="timeseries.soil.otus.dna.always" sheetId="2" r:id="rId7"/>
+    <sheet name="timeseries.soil.otus.dna.blips" sheetId="4" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="Slicer_Pattern">#N/A</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId9"/>
+    <pivotCache cacheId="0" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -1853,14 +1853,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3888,10 +3887,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="45258.895760416664" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="567" xr:uid="{75980933-70FD-4C44-AAB6-FD3050B14EE6}">
   <cacheSource type="worksheet">
@@ -6194,7 +6189,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AE418AD6-7E9F-1343-B5E6-5A67034D120A}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AE418AD6-7E9F-1343-B5E6-5A67034D120A}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:H3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField dataField="1" showAll="0"/>
@@ -6364,9 +6359,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6404,7 +6399,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -6510,7 +6505,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6652,7 +6647,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6662,7 +6657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B29CBC95-9131-244E-B52A-04C012EAC939}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="174" workbookViewId="0"/>
+    <sheetView zoomScale="174" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6709,25 +6704,25 @@
       <c r="A3" t="s">
         <v>575</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3">
         <v>55</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3">
         <v>465</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3">
         <v>8</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3">
         <v>15</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3">
         <v>22</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3">
         <v>567</v>
       </c>
     </row>
@@ -6748,7 +6743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2748E6D-9BB8-804B-B244-BF5F8D0D3FDE}">
   <dimension ref="A1:B568"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="135" workbookViewId="0">
+    <sheetView zoomScale="135" workbookViewId="0">
       <selection activeCell="A547" sqref="A547:A568"/>
     </sheetView>
   </sheetViews>
@@ -11918,8 +11913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B117A00-495A-9E42-90CC-453539EB2081}">
   <dimension ref="A1:A466"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>